<commit_message>
xml conversion has been completed
</commit_message>
<xml_diff>
--- a/MyFirstExcel.xlsx
+++ b/MyFirstExcel.xlsx
@@ -585,9 +585,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -700,9 +707,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7399,8 +7415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>